<commit_message>
Added assign functions, added timetabletester.
</commit_message>
<xml_diff>
--- a/lecture_times.xlsx
+++ b/lecture_times.xlsx
@@ -61562,16 +61562,16 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>3057</v>
+        <v>3056</v>
       </c>
       <c r="C7" t="s">
-        <v>3073</v>
+        <v>3072</v>
       </c>
       <c r="D7" t="s">
-        <v>3082</v>
+        <v>3083</v>
       </c>
       <c r="E7" t="s">
-        <v>3092</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -61579,16 +61579,16 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>3056</v>
+        <v>3054</v>
       </c>
       <c r="C8" t="s">
-        <v>3072</v>
+        <v>3070</v>
       </c>
       <c r="D8" t="s">
-        <v>3083</v>
+        <v>3082</v>
       </c>
       <c r="E8" t="s">
-        <v>3089</v>
+        <v>3088</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -61596,16 +61596,16 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>3054</v>
+        <v>3057</v>
       </c>
       <c r="C9" t="s">
-        <v>3070</v>
+        <v>3073</v>
       </c>
       <c r="D9" t="s">
         <v>3082</v>
       </c>
       <c r="E9" t="s">
-        <v>3088</v>
+        <v>3092</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -61613,16 +61613,16 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>3058</v>
+        <v>3061</v>
       </c>
       <c r="C10" t="s">
-        <v>3074</v>
+        <v>3077</v>
       </c>
       <c r="D10" t="s">
         <v>3084</v>
       </c>
       <c r="E10" t="s">
-        <v>3091</v>
+        <v>3092</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -61664,16 +61664,16 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>3061</v>
+        <v>3058</v>
       </c>
       <c r="C13" t="s">
-        <v>3077</v>
+        <v>3074</v>
       </c>
       <c r="D13" t="s">
         <v>3084</v>
       </c>
       <c r="E13" t="s">
-        <v>3092</v>
+        <v>3091</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -61681,16 +61681,16 @@
         <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>3065</v>
+        <v>3062</v>
       </c>
       <c r="C14" t="s">
-        <v>3081</v>
+        <v>3078</v>
       </c>
       <c r="D14" t="s">
         <v>3083</v>
       </c>
       <c r="E14" t="s">
-        <v>3092</v>
+        <v>3087</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -61698,16 +61698,16 @@
         <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>3064</v>
+        <v>3063</v>
       </c>
       <c r="C15" t="s">
-        <v>3080</v>
+        <v>3079</v>
       </c>
       <c r="D15" t="s">
         <v>3082</v>
       </c>
       <c r="E15" t="s">
-        <v>3089</v>
+        <v>3091</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -61715,16 +61715,16 @@
         <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>3062</v>
+        <v>3064</v>
       </c>
       <c r="C16" t="s">
-        <v>3078</v>
+        <v>3080</v>
       </c>
       <c r="D16" t="s">
-        <v>3083</v>
+        <v>3082</v>
       </c>
       <c r="E16" t="s">
-        <v>3087</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -61732,16 +61732,16 @@
         <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>3063</v>
+        <v>3065</v>
       </c>
       <c r="C17" t="s">
-        <v>3079</v>
+        <v>3081</v>
       </c>
       <c r="D17" t="s">
-        <v>3082</v>
+        <v>3083</v>
       </c>
       <c r="E17" t="s">
-        <v>3091</v>
+        <v>3092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>